<commit_message>
Correct typo for RPA1 SMYD4
</commit_message>
<xml_diff>
--- a/output/finalPromoterGDOa30.xlsx
+++ b/output/finalPromoterGDOa30.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjpl\Documents\GitHub\CRISPR-Library-Design\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF78FA5-847D-4DC8-B0E5-3E4050E50670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A71DDA-9AF9-4AA1-AFFE-8E1D0F39484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10850" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="19090" yWindow="-10850" windowWidth="38620" windowHeight="21100" xr2:uid="{2633FF3E-BE28-4DDF-9783-64AD6AA4D79B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2633FF3E-BE28-4DDF-9783-64AD6AA4D79B}"/>
   </bookViews>
   <sheets>
     <sheet name="Final" sheetId="2" r:id="rId1"/>
@@ -449,13 +449,13 @@
     <t>&lt;picked</t>
   </si>
   <si>
-    <t>RAP1-SMYD4</t>
-  </si>
-  <si>
     <t>GCGCTACGCAGCCGCCGCAT</t>
   </si>
   <si>
     <t>UCSC Genome Browser.. Start bp</t>
+  </si>
+  <si>
+    <t>RPA1|SMYD4</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="E36" sqref="E36"/>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B20" t="s">
         <v>57</v>
@@ -1540,7 +1540,7 @@
         <v>58</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B21" t="s">
         <v>57</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B22" t="s">
         <v>57</v>
@@ -4185,7 +4185,7 @@
         <v>49</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.3">

</xml_diff>